<commit_message>
add chart in excel
</commit_message>
<xml_diff>
--- a/docs/WDCP.xlsx
+++ b/docs/WDCP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,6 +81,34 @@
   </si>
   <si>
     <t>FAILED_SSL_REQUIRED_BY_SERVER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>request_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_TYPE_AP_LIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前设备检测到的AP列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_TYPE_BASIC_INFO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前设备基本信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C8"/>
+      <selection activeCell="C12" sqref="A10:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -505,6 +533,39 @@
       </c>
       <c r="C8" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data request handle
</commit_message>
<xml_diff>
--- a/docs/WDCP.xlsx
+++ b/docs/WDCP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAILED_AUTH_CHECK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份验证错误</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="A10:C12"/>
+      <selection activeCell="A10" sqref="A10:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -537,7 +549,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -548,23 +560,56 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change wdcp, add fake ap request and response
</commit_message>
<xml_diff>
--- a/docs/WDCP.xlsx
+++ b/docs/WDCP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,6 +168,17 @@
   </si>
   <si>
     <t>采用WPA加密</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_TYPE_FAKE_AP</t>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前存在FakeAP威胁的AP的信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -517,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -664,47 +675,58 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add flow statisitics in wdcp
</commit_message>
<xml_diff>
--- a/docs/WDCP.xlsx
+++ b/docs/WDCP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,6 +179,18 @@
   </si>
   <si>
     <t>获取当前存在FakeAP威胁的AP的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ_TYPE_FLOW_STATISTICS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取当前设备统计的数据流量信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -686,47 +698,58 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>